<commit_message>
Resolving Tumour Size issue
</commit_message>
<xml_diff>
--- a/CancerSummary/SummaryReports.xlsx
+++ b/CancerSummary/SummaryReports.xlsx
@@ -516,37 +516,37 @@
         <v>100</v>
       </c>
       <c r="C2" t="n">
-        <v>34629</v>
+        <v>35202</v>
       </c>
       <c r="D2" t="n">
         <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>10073</v>
+        <v>10561</v>
       </c>
       <c r="F2" t="n">
         <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>5418</v>
+        <v>5427</v>
       </c>
       <c r="H2" t="n">
         <v>100</v>
       </c>
       <c r="I2" t="n">
-        <v>6666</v>
+        <v>6681</v>
       </c>
       <c r="J2" t="n">
         <v>100</v>
       </c>
       <c r="K2" t="n">
-        <v>7447</v>
+        <v>7484</v>
       </c>
       <c r="L2" t="n">
         <v>100</v>
       </c>
       <c r="M2" t="n">
-        <v>5025</v>
+        <v>5049</v>
       </c>
     </row>
     <row r="3">
@@ -559,37 +559,37 @@
         <v>94.81999999999999</v>
       </c>
       <c r="C3" t="n">
-        <v>32834</v>
+        <v>33380</v>
       </c>
       <c r="D3" t="n">
-        <v>94.73999999999999</v>
+        <v>94.70999999999999</v>
       </c>
       <c r="E3" t="n">
-        <v>9543</v>
+        <v>10002</v>
       </c>
       <c r="F3" t="n">
-        <v>95.42</v>
+        <v>95.48999999999999</v>
       </c>
       <c r="G3" t="n">
-        <v>5170</v>
+        <v>5182</v>
       </c>
       <c r="H3" t="n">
-        <v>95.81</v>
+        <v>95.84</v>
       </c>
       <c r="I3" t="n">
-        <v>6387</v>
+        <v>6403</v>
       </c>
       <c r="J3" t="n">
-        <v>94.31999999999999</v>
+        <v>94.36</v>
       </c>
       <c r="K3" t="n">
-        <v>7024</v>
+        <v>7062</v>
       </c>
       <c r="L3" t="n">
-        <v>93.73</v>
+        <v>93.7</v>
       </c>
       <c r="M3" t="n">
-        <v>4710</v>
+        <v>4731</v>
       </c>
     </row>
     <row r="4">
@@ -602,37 +602,37 @@
         <v>100</v>
       </c>
       <c r="C4" t="n">
-        <v>34629</v>
+        <v>35202</v>
       </c>
       <c r="D4" t="n">
         <v>100</v>
       </c>
       <c r="E4" t="n">
-        <v>10073</v>
+        <v>10561</v>
       </c>
       <c r="F4" t="n">
         <v>100</v>
       </c>
       <c r="G4" t="n">
-        <v>5418</v>
+        <v>5427</v>
       </c>
       <c r="H4" t="n">
         <v>100</v>
       </c>
       <c r="I4" t="n">
-        <v>6666</v>
+        <v>6681</v>
       </c>
       <c r="J4" t="n">
         <v>100</v>
       </c>
       <c r="K4" t="n">
-        <v>7447</v>
+        <v>7484</v>
       </c>
       <c r="L4" t="n">
         <v>100</v>
       </c>
       <c r="M4" t="n">
-        <v>5025</v>
+        <v>5049</v>
       </c>
     </row>
     <row r="5">
@@ -645,37 +645,37 @@
         <v>100</v>
       </c>
       <c r="C5" t="n">
-        <v>34629</v>
+        <v>35202</v>
       </c>
       <c r="D5" t="n">
         <v>100</v>
       </c>
       <c r="E5" t="n">
-        <v>10073</v>
+        <v>10561</v>
       </c>
       <c r="F5" t="n">
         <v>100</v>
       </c>
       <c r="G5" t="n">
-        <v>5418</v>
+        <v>5427</v>
       </c>
       <c r="H5" t="n">
         <v>100</v>
       </c>
       <c r="I5" t="n">
-        <v>6666</v>
+        <v>6681</v>
       </c>
       <c r="J5" t="n">
         <v>100</v>
       </c>
       <c r="K5" t="n">
-        <v>7447</v>
+        <v>7484</v>
       </c>
       <c r="L5" t="n">
         <v>100</v>
       </c>
       <c r="M5" t="n">
-        <v>5025</v>
+        <v>5049</v>
       </c>
     </row>
     <row r="6">
@@ -688,37 +688,37 @@
         <v>100</v>
       </c>
       <c r="C6" t="n">
-        <v>34629</v>
+        <v>35202</v>
       </c>
       <c r="D6" t="n">
         <v>100</v>
       </c>
       <c r="E6" t="n">
-        <v>10073</v>
+        <v>10561</v>
       </c>
       <c r="F6" t="n">
         <v>100</v>
       </c>
       <c r="G6" t="n">
-        <v>5418</v>
+        <v>5427</v>
       </c>
       <c r="H6" t="n">
         <v>100</v>
       </c>
       <c r="I6" t="n">
-        <v>6666</v>
+        <v>6681</v>
       </c>
       <c r="J6" t="n">
         <v>100</v>
       </c>
       <c r="K6" t="n">
-        <v>7447</v>
+        <v>7484</v>
       </c>
       <c r="L6" t="n">
         <v>100</v>
       </c>
       <c r="M6" t="n">
-        <v>5025</v>
+        <v>5049</v>
       </c>
     </row>
     <row r="7">
@@ -728,40 +728,40 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>99.13</v>
+        <v>99.14</v>
       </c>
       <c r="C7" t="n">
-        <v>34328</v>
+        <v>34901</v>
       </c>
       <c r="D7" t="n">
-        <v>98.64</v>
+        <v>98.7</v>
       </c>
       <c r="E7" t="n">
-        <v>9936</v>
+        <v>10424</v>
       </c>
       <c r="F7" t="n">
         <v>99.02</v>
       </c>
       <c r="G7" t="n">
-        <v>5365</v>
+        <v>5374</v>
       </c>
       <c r="H7" t="n">
-        <v>99.26000000000001</v>
+        <v>99.27</v>
       </c>
       <c r="I7" t="n">
-        <v>6617</v>
+        <v>6632</v>
       </c>
       <c r="J7" t="n">
         <v>99.48999999999999</v>
       </c>
       <c r="K7" t="n">
-        <v>7409</v>
+        <v>7446</v>
       </c>
       <c r="L7" t="n">
         <v>99.52</v>
       </c>
       <c r="M7" t="n">
-        <v>5001</v>
+        <v>5025</v>
       </c>
     </row>
     <row r="8">
@@ -774,37 +774,37 @@
         <v>100</v>
       </c>
       <c r="C8" t="n">
-        <v>34629</v>
+        <v>35202</v>
       </c>
       <c r="D8" t="n">
         <v>100</v>
       </c>
       <c r="E8" t="n">
-        <v>10073</v>
+        <v>10561</v>
       </c>
       <c r="F8" t="n">
         <v>100</v>
       </c>
       <c r="G8" t="n">
-        <v>5418</v>
+        <v>5427</v>
       </c>
       <c r="H8" t="n">
         <v>100</v>
       </c>
       <c r="I8" t="n">
-        <v>6666</v>
+        <v>6681</v>
       </c>
       <c r="J8" t="n">
         <v>100</v>
       </c>
       <c r="K8" t="n">
-        <v>7447</v>
+        <v>7484</v>
       </c>
       <c r="L8" t="n">
         <v>100</v>
       </c>
       <c r="M8" t="n">
-        <v>5025</v>
+        <v>5049</v>
       </c>
     </row>
     <row r="9">
@@ -814,40 +814,40 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>83.33</v>
+        <v>82.40000000000001</v>
       </c>
       <c r="C9" t="n">
-        <v>28856</v>
+        <v>29008</v>
       </c>
       <c r="D9" t="n">
-        <v>68.26000000000001</v>
+        <v>65.20999999999999</v>
       </c>
       <c r="E9" t="n">
-        <v>6876</v>
+        <v>6887</v>
       </c>
       <c r="F9" t="n">
-        <v>87.97</v>
+        <v>88.23999999999999</v>
       </c>
       <c r="G9" t="n">
-        <v>4766</v>
+        <v>4789</v>
       </c>
       <c r="H9" t="n">
-        <v>89.62</v>
+        <v>89.79000000000001</v>
       </c>
       <c r="I9" t="n">
-        <v>5974</v>
+        <v>5999</v>
       </c>
       <c r="J9" t="n">
-        <v>92.18000000000001</v>
+        <v>92.54000000000001</v>
       </c>
       <c r="K9" t="n">
-        <v>6865</v>
+        <v>6926</v>
       </c>
       <c r="L9" t="n">
-        <v>87.06</v>
+        <v>87.28</v>
       </c>
       <c r="M9" t="n">
-        <v>4375</v>
+        <v>4407</v>
       </c>
     </row>
     <row r="10">
@@ -857,40 +857,40 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>29.73</v>
+        <v>29.88</v>
       </c>
       <c r="C10" t="n">
-        <v>10295</v>
+        <v>10518</v>
       </c>
       <c r="D10" t="n">
-        <v>29.92</v>
+        <v>28.55</v>
       </c>
       <c r="E10" t="n">
-        <v>3014</v>
+        <v>3015</v>
       </c>
       <c r="F10" t="n">
-        <v>36.93</v>
+        <v>37.44</v>
       </c>
       <c r="G10" t="n">
-        <v>2001</v>
+        <v>2032</v>
       </c>
       <c r="H10" t="n">
-        <v>33.08</v>
+        <v>34.1</v>
       </c>
       <c r="I10" t="n">
-        <v>2205</v>
+        <v>2278</v>
       </c>
       <c r="J10" t="n">
-        <v>26.98</v>
+        <v>27.9</v>
       </c>
       <c r="K10" t="n">
-        <v>2009</v>
+        <v>2088</v>
       </c>
       <c r="L10" t="n">
-        <v>21.21</v>
+        <v>21.89</v>
       </c>
       <c r="M10" t="n">
-        <v>1066</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="11">
@@ -900,40 +900,40 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>49.77</v>
+        <v>49.4</v>
       </c>
       <c r="C11" t="n">
-        <v>17236</v>
+        <v>17390</v>
       </c>
       <c r="D11" t="n">
-        <v>49.51</v>
+        <v>48.24</v>
       </c>
       <c r="E11" t="n">
-        <v>4987</v>
+        <v>5095</v>
       </c>
       <c r="F11" t="n">
-        <v>48.74</v>
+        <v>48.65</v>
       </c>
       <c r="G11" t="n">
-        <v>2641</v>
+        <v>2640</v>
       </c>
       <c r="H11" t="n">
-        <v>53.15</v>
+        <v>53.09</v>
       </c>
       <c r="I11" t="n">
-        <v>3543</v>
+        <v>3547</v>
       </c>
       <c r="J11" t="n">
-        <v>53.62</v>
+        <v>53.74</v>
       </c>
       <c r="K11" t="n">
-        <v>3993</v>
+        <v>4022</v>
       </c>
       <c r="L11" t="n">
-        <v>41.23</v>
+        <v>41.32</v>
       </c>
       <c r="M11" t="n">
-        <v>2072</v>
+        <v>2086</v>
       </c>
     </row>
   </sheetData>
@@ -1029,40 +1029,40 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>58.92</v>
+        <v>58.9</v>
       </c>
       <c r="C2" t="n">
-        <v>7890</v>
+        <v>7883</v>
       </c>
       <c r="D2" t="n">
-        <v>31.69</v>
+        <v>31.7</v>
       </c>
       <c r="E2" t="n">
         <v>1751</v>
       </c>
       <c r="F2" t="n">
-        <v>69.41</v>
+        <v>69.37</v>
       </c>
       <c r="G2" t="n">
-        <v>1613</v>
+        <v>1610</v>
       </c>
       <c r="H2" t="n">
-        <v>84.87</v>
+        <v>84.84999999999999</v>
       </c>
       <c r="I2" t="n">
-        <v>1823</v>
+        <v>1820</v>
       </c>
       <c r="J2" t="n">
-        <v>80.7</v>
+        <v>80.68000000000001</v>
       </c>
       <c r="K2" t="n">
-        <v>1681</v>
+        <v>1679</v>
       </c>
       <c r="L2" t="n">
-        <v>77.90000000000001</v>
+        <v>77.91</v>
       </c>
       <c r="M2" t="n">
-        <v>1022</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="3">
@@ -1075,37 +1075,37 @@
         <v>34.45</v>
       </c>
       <c r="C3" t="n">
-        <v>4613</v>
+        <v>4611</v>
       </c>
       <c r="D3" t="n">
-        <v>8.43</v>
+        <v>8.44</v>
       </c>
       <c r="E3" t="n">
         <v>466</v>
       </c>
       <c r="F3" t="n">
-        <v>42.08</v>
+        <v>42.09</v>
       </c>
       <c r="G3" t="n">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="H3" t="n">
-        <v>55.45</v>
+        <v>55.48</v>
       </c>
       <c r="I3" t="n">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="J3" t="n">
         <v>56.46</v>
       </c>
       <c r="K3" t="n">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="L3" t="n">
-        <v>61.13</v>
+        <v>61.16</v>
       </c>
       <c r="M3" t="n">
-        <v>802</v>
+        <v>803</v>
       </c>
     </row>
     <row r="4">
@@ -1115,40 +1115,40 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>48.65</v>
+        <v>48.64</v>
       </c>
       <c r="C4" t="n">
-        <v>6515</v>
+        <v>6510</v>
       </c>
       <c r="D4" t="n">
-        <v>19.49</v>
+        <v>19.5</v>
       </c>
       <c r="E4" t="n">
         <v>1077</v>
       </c>
       <c r="F4" t="n">
-        <v>55.59</v>
+        <v>55.58</v>
       </c>
       <c r="G4" t="n">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="H4" t="n">
-        <v>77.09</v>
+        <v>77.11</v>
       </c>
       <c r="I4" t="n">
-        <v>1656</v>
+        <v>1654</v>
       </c>
       <c r="J4" t="n">
-        <v>75.28</v>
+        <v>75.25</v>
       </c>
       <c r="K4" t="n">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="L4" t="n">
-        <v>70.27</v>
+        <v>70.3</v>
       </c>
       <c r="M4" t="n">
-        <v>922</v>
+        <v>923</v>
       </c>
     </row>
     <row r="5">
@@ -1158,7 +1158,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.23</v>
+        <v>3.24</v>
       </c>
       <c r="C5" t="n">
         <v>433</v>
@@ -1176,13 +1176,13 @@
         <v>89</v>
       </c>
       <c r="H5" t="n">
-        <v>7.77</v>
+        <v>7.79</v>
       </c>
       <c r="I5" t="n">
         <v>167</v>
       </c>
       <c r="J5" t="n">
-        <v>6.96</v>
+        <v>6.97</v>
       </c>
       <c r="K5" t="n">
         <v>145</v>
@@ -1225,7 +1225,7 @@
         <v>36</v>
       </c>
       <c r="J6" t="n">
-        <v>3.02</v>
+        <v>3.03</v>
       </c>
       <c r="K6" t="n">
         <v>63</v>
@@ -1244,37 +1244,37 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>59.26</v>
+        <v>59.25</v>
       </c>
       <c r="C7" t="n">
-        <v>7936</v>
+        <v>7929</v>
       </c>
       <c r="D7" t="n">
-        <v>41.01</v>
+        <v>40.99</v>
       </c>
       <c r="E7" t="n">
-        <v>2266</v>
+        <v>2264</v>
       </c>
       <c r="F7" t="n">
-        <v>65.88</v>
+        <v>65.83</v>
       </c>
       <c r="G7" t="n">
-        <v>1531</v>
+        <v>1528</v>
       </c>
       <c r="H7" t="n">
-        <v>70.95</v>
+        <v>71</v>
       </c>
       <c r="I7" t="n">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="J7" t="n">
-        <v>74.56</v>
+        <v>74.58</v>
       </c>
       <c r="K7" t="n">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="L7" t="n">
-        <v>80.95</v>
+        <v>80.88</v>
       </c>
       <c r="M7" t="n">
         <v>1062</v>
@@ -1287,37 +1287,37 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>55.76</v>
+        <v>55.8</v>
       </c>
       <c r="C8" t="n">
         <v>7468</v>
       </c>
       <c r="D8" t="n">
-        <v>36.78</v>
+        <v>36.79</v>
       </c>
       <c r="E8" t="n">
         <v>2032</v>
       </c>
       <c r="F8" t="n">
-        <v>62.69</v>
+        <v>62.77</v>
       </c>
       <c r="G8" t="n">
         <v>1457</v>
       </c>
       <c r="H8" t="n">
-        <v>66.84999999999999</v>
+        <v>66.95</v>
       </c>
       <c r="I8" t="n">
         <v>1436</v>
       </c>
       <c r="J8" t="n">
-        <v>71.63</v>
+        <v>71.7</v>
       </c>
       <c r="K8" t="n">
         <v>1492</v>
       </c>
       <c r="L8" t="n">
-        <v>80.11</v>
+        <v>80.05</v>
       </c>
       <c r="M8" t="n">
         <v>1051</v>
@@ -1333,37 +1333,37 @@
         <v>99.13</v>
       </c>
       <c r="C9" t="n">
-        <v>13275</v>
+        <v>13266</v>
       </c>
       <c r="D9" t="n">
         <v>98.91</v>
       </c>
       <c r="E9" t="n">
-        <v>5465</v>
+        <v>5463</v>
       </c>
       <c r="F9" t="n">
-        <v>99.23</v>
+        <v>99.22</v>
       </c>
       <c r="G9" t="n">
-        <v>2306</v>
+        <v>2303</v>
       </c>
       <c r="H9" t="n">
-        <v>98.84</v>
+        <v>98.83</v>
       </c>
       <c r="I9" t="n">
-        <v>2123</v>
+        <v>2120</v>
       </c>
       <c r="J9" t="n">
         <v>99.56999999999999</v>
       </c>
       <c r="K9" t="n">
-        <v>2074</v>
+        <v>2072</v>
       </c>
       <c r="L9" t="n">
         <v>99.62</v>
       </c>
       <c r="M9" t="n">
-        <v>1307</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="10">
@@ -1376,37 +1376,37 @@
         <v>56.7</v>
       </c>
       <c r="C10" t="n">
-        <v>7593</v>
+        <v>7588</v>
       </c>
       <c r="D10" t="n">
-        <v>37.14</v>
+        <v>37.15</v>
       </c>
       <c r="E10" t="n">
         <v>2052</v>
       </c>
       <c r="F10" t="n">
-        <v>52.15</v>
+        <v>52.09</v>
       </c>
       <c r="G10" t="n">
-        <v>1212</v>
+        <v>1209</v>
       </c>
       <c r="H10" t="n">
-        <v>73.14</v>
+        <v>73.15000000000001</v>
       </c>
       <c r="I10" t="n">
-        <v>1571</v>
+        <v>1569</v>
       </c>
       <c r="J10" t="n">
-        <v>81.95</v>
+        <v>81.98</v>
       </c>
       <c r="K10" t="n">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="L10" t="n">
-        <v>80.11</v>
+        <v>80.12</v>
       </c>
       <c r="M10" t="n">
-        <v>1051</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="11">
@@ -1419,37 +1419,37 @@
         <v>53.52</v>
       </c>
       <c r="C11" t="n">
-        <v>7168</v>
+        <v>7163</v>
       </c>
       <c r="D11" t="n">
-        <v>34.82</v>
+        <v>34.84</v>
       </c>
       <c r="E11" t="n">
         <v>1924</v>
       </c>
       <c r="F11" t="n">
-        <v>50.17</v>
+        <v>50.11</v>
       </c>
       <c r="G11" t="n">
-        <v>1166</v>
+        <v>1163</v>
       </c>
       <c r="H11" t="n">
-        <v>70.11</v>
+        <v>70.12</v>
       </c>
       <c r="I11" t="n">
-        <v>1506</v>
+        <v>1504</v>
       </c>
       <c r="J11" t="n">
-        <v>76.62</v>
+        <v>76.65000000000001</v>
       </c>
       <c r="K11" t="n">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="L11" t="n">
-        <v>74.39</v>
+        <v>74.41</v>
       </c>
       <c r="M11" t="n">
-        <v>976</v>
+        <v>977</v>
       </c>
     </row>
     <row r="12">
@@ -1459,37 +1459,37 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>40.29</v>
+        <v>40.27</v>
       </c>
       <c r="C12" t="n">
-        <v>5395</v>
+        <v>5389</v>
       </c>
       <c r="D12" t="n">
-        <v>25.7</v>
+        <v>25.71</v>
       </c>
       <c r="E12" t="n">
         <v>1420</v>
       </c>
       <c r="F12" t="n">
-        <v>37.26</v>
+        <v>37.18</v>
       </c>
       <c r="G12" t="n">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="H12" t="n">
-        <v>49.07</v>
+        <v>49.04</v>
       </c>
       <c r="I12" t="n">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="J12" t="n">
-        <v>58.04</v>
+        <v>58.05</v>
       </c>
       <c r="K12" t="n">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="L12" t="n">
-        <v>64.48</v>
+        <v>64.43000000000001</v>
       </c>
       <c r="M12" t="n">
         <v>846</v>
@@ -1502,40 +1502,40 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>62.77</v>
+        <v>64.31</v>
       </c>
       <c r="C13" t="n">
-        <v>8406</v>
+        <v>8607</v>
       </c>
       <c r="D13" t="n">
-        <v>50.12</v>
+        <v>50.15</v>
       </c>
       <c r="E13" t="n">
-        <v>2769</v>
+        <v>2770</v>
       </c>
       <c r="F13" t="n">
-        <v>73.23999999999999</v>
+        <v>74.62</v>
       </c>
       <c r="G13" t="n">
-        <v>1702</v>
+        <v>1732</v>
       </c>
       <c r="H13" t="n">
-        <v>77.42</v>
+        <v>80.75</v>
       </c>
       <c r="I13" t="n">
-        <v>1663</v>
+        <v>1732</v>
       </c>
       <c r="J13" t="n">
-        <v>70.19</v>
+        <v>73.43000000000001</v>
       </c>
       <c r="K13" t="n">
-        <v>1462</v>
+        <v>1528</v>
       </c>
       <c r="L13" t="n">
-        <v>61.74</v>
+        <v>64.36</v>
       </c>
       <c r="M13" t="n">
-        <v>810</v>
+        <v>845</v>
       </c>
     </row>
     <row r="14">
@@ -1545,37 +1545,37 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>49.31</v>
+        <v>49.3</v>
       </c>
       <c r="C14" t="n">
-        <v>6603</v>
+        <v>6598</v>
       </c>
       <c r="D14" t="n">
-        <v>36.63</v>
+        <v>36.61</v>
       </c>
       <c r="E14" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="F14" t="n">
-        <v>57.1</v>
+        <v>57.13</v>
       </c>
       <c r="G14" t="n">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="H14" t="n">
-        <v>61.17</v>
+        <v>61.21</v>
       </c>
       <c r="I14" t="n">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="J14" t="n">
-        <v>58.86</v>
+        <v>58.87</v>
       </c>
       <c r="K14" t="n">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="L14" t="n">
-        <v>54.27</v>
+        <v>54.23</v>
       </c>
       <c r="M14" t="n">
         <v>712</v>
@@ -1588,37 +1588,37 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>52.77</v>
+        <v>52.76</v>
       </c>
       <c r="C15" t="n">
-        <v>7067</v>
+        <v>7061</v>
       </c>
       <c r="D15" t="n">
-        <v>39.67</v>
+        <v>39.65</v>
       </c>
       <c r="E15" t="n">
-        <v>2192</v>
+        <v>2190</v>
       </c>
       <c r="F15" t="n">
         <v>65.09999999999999</v>
       </c>
       <c r="G15" t="n">
-        <v>1513</v>
+        <v>1511</v>
       </c>
       <c r="H15" t="n">
-        <v>64.34</v>
+        <v>64.38</v>
       </c>
       <c r="I15" t="n">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="J15" t="n">
-        <v>60.73</v>
+        <v>60.74</v>
       </c>
       <c r="K15" t="n">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="L15" t="n">
-        <v>54.5</v>
+        <v>54.46</v>
       </c>
       <c r="M15" t="n">
         <v>715</v>
@@ -1635,7 +1635,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1668,238 +1668,238 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>NMSC</t>
+          <t>Bone and Articular Cartilage</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6680</v>
+        <v>20</v>
       </c>
       <c r="C2" t="n">
-        <v>94</v>
+        <v>3</v>
       </c>
       <c r="D2" t="n">
-        <v>347</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>bladder</t>
+          <t>NMSC</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>121</v>
+        <v>6681</v>
       </c>
       <c r="C3" t="n">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>347</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>brain, CNS</t>
+          <t>Nasal cavity, middle ear, sinuses</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>167</v>
+        <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>cervix uteri</t>
+          <t>bladder</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>175</v>
+        <v>121</v>
       </c>
       <c r="C5" t="n">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D5" t="n">
-        <v>51</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>colorectal cancer</t>
+          <t>bowel</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1398</v>
+        <v>61</v>
       </c>
       <c r="C6" t="n">
-        <v>959</v>
+        <v>41</v>
       </c>
       <c r="D6" t="n">
-        <v>171</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>corpus uteri</t>
+          <t>brain, CNS</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>707</v>
+        <v>167</v>
       </c>
       <c r="C7" t="n">
-        <v>572</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>120</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>female breast</t>
+          <t>breast</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>9891</v>
+        <v>9950</v>
       </c>
       <c r="C8" t="n">
-        <v>8214</v>
+        <v>8205</v>
       </c>
       <c r="D8" t="n">
-        <v>7703</v>
+        <v>7904</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>gallbladder</t>
+          <t>cervix uteri</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="C9" t="n">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>hodgkin lymphoma</t>
+          <t>colorectal cancer</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>62</v>
+        <v>1398</v>
       </c>
       <c r="C10" t="n">
-        <v>44</v>
+        <v>959</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>hypopharynx</t>
+          <t>corpus uteri</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>3</v>
+        <v>707</v>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>572</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>in-situ</t>
+          <t>gallbladder</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4567</v>
+        <v>29</v>
       </c>
       <c r="C12" t="n">
-        <v>4132</v>
+        <v>21</v>
       </c>
       <c r="D12" t="n">
-        <v>811</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>kaposi sarcoma</t>
+          <t>hodgkin lymphoma</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>kidney</t>
+          <t>hypopharynx</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>246</v>
+        <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>153</v>
+        <v>2</v>
       </c>
       <c r="D14" t="n">
-        <v>134</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>larynx</t>
+          <t>in-situ</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>5</v>
+        <v>4567</v>
       </c>
       <c r="C15" t="n">
-        <v>4</v>
+        <v>4241</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>812</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>leukemia</t>
+          <t>kaposi sarcoma</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>255</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
@@ -1908,288 +1908,336 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>lip</t>
+          <t>kidney</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>112</v>
+        <v>246</v>
       </c>
       <c r="C17" t="n">
-        <v>74</v>
+        <v>153</v>
       </c>
       <c r="D17" t="n">
-        <v>52</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>liver</t>
+          <t>larynx</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>73</v>
+        <v>5</v>
       </c>
       <c r="C18" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D18" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>lung</t>
+          <t>leukemia</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>582</v>
+        <v>255</v>
       </c>
       <c r="C19" t="n">
-        <v>487</v>
+        <v>33</v>
       </c>
       <c r="D19" t="n">
-        <v>234</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>melanoma of skin</t>
+          <t>lip, oral cavity</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1176</v>
+        <v>112</v>
       </c>
       <c r="C20" t="n">
-        <v>829</v>
+        <v>74</v>
       </c>
       <c r="D20" t="n">
-        <v>324</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>mesothelioma</t>
+          <t>liver</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="C21" t="n">
+        <v>25</v>
+      </c>
+      <c r="D21" t="n">
         <v>15</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>multiple myeloma</t>
+          <t>lung</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>184</v>
+        <v>582</v>
       </c>
       <c r="C22" t="n">
-        <v>30</v>
+        <v>487</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>234</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>nasopharynx</t>
+          <t>melanoma of skin</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>4</v>
+        <v>1176</v>
       </c>
       <c r="C23" t="n">
-        <v>3</v>
+        <v>829</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>324</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>non-Hodgkin lymphoma</t>
+          <t>mesothelioma</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>484</v>
+        <v>28</v>
       </c>
       <c r="C24" t="n">
-        <v>325</v>
+        <v>15</v>
       </c>
       <c r="D24" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>oesophagus</t>
+          <t>multiple myeloma</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>114</v>
+        <v>184</v>
       </c>
       <c r="C25" t="n">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="D25" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>oropharynx</t>
+          <t>nasopharynx</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="C26" t="n">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="D26" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>ovary</t>
+          <t>non-Hodgkin lymphoma</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>648</v>
+        <v>484</v>
       </c>
       <c r="C27" t="n">
-        <v>505</v>
+        <v>325</v>
       </c>
       <c r="D27" t="n">
-        <v>53</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>pancreas</t>
+          <t>oesophagus</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>245</v>
+        <v>114</v>
       </c>
       <c r="C28" t="n">
-        <v>157</v>
+        <v>64</v>
       </c>
       <c r="D28" t="n">
-        <v>65</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>salivary glands</t>
+          <t>oropharynx</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C29" t="n">
+        <v>27</v>
+      </c>
+      <c r="D29" t="n">
         <v>10</v>
-      </c>
-      <c r="D29" t="n">
-        <v>12</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>stomach</t>
+          <t>ovary</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>91</v>
+        <v>648</v>
       </c>
       <c r="C30" t="n">
-        <v>54</v>
+        <v>505</v>
       </c>
       <c r="D30" t="n">
-        <v>16</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>thyroid</t>
+          <t>pancreas</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C31" t="n">
-        <v>80</v>
+        <v>157</v>
       </c>
       <c r="D31" t="n">
-        <v>108</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>unknown/uncertain</t>
+          <t>salivary glands</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>441</v>
+        <v>26</v>
       </c>
       <c r="C32" t="n">
-        <v>131</v>
+        <v>10</v>
       </c>
       <c r="D32" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>vagina</t>
+          <t>stomach</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="C33" t="n">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>thyroid</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>243</v>
+      </c>
+      <c r="C34" t="n">
+        <v>80</v>
+      </c>
+      <c r="D34" t="n">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>unknown/uncertain</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>441</v>
+      </c>
+      <c r="C35" t="n">
+        <v>131</v>
+      </c>
+      <c r="D35" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>vagina</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>12</v>
+      </c>
+      <c r="C36" t="n">
+        <v>5</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
           <t>vulva</t>
         </is>
       </c>
-      <c r="B34" t="n">
+      <c r="B37" t="n">
         <v>51</v>
       </c>
-      <c r="C34" t="n">
+      <c r="C37" t="n">
         <v>23</v>
       </c>
-      <c r="D34" t="n">
+      <c r="D37" t="n">
         <v>23</v>
       </c>
     </row>
@@ -2204,7 +2252,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2227,330 +2275,360 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>NMSC</t>
+          <t>Bone and Articular Cartilage</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7777</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>bladder</t>
+          <t>NMSC</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>145</v>
+        <v>7779</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>brain, CNS</t>
+          <t>Nasal cavity, middle ear, sinuses</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>198</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>cervix uteri</t>
+          <t>bladder</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>281</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>colorectal cancer</t>
+          <t>bowel</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1616</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>corpus uteri</t>
+          <t>brain, CNS</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>806</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>female breast</t>
+          <t>breast</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>11599</v>
+        <v>11590</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>gallbladder</t>
+          <t>cervix uteri</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>33</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>hodgkin lymphoma</t>
+          <t>colorectal cancer</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>131</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>hypopharynx</t>
+          <t>corpus uteri</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4</v>
+        <v>806</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>in-situ</t>
+          <t>gallbladder</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5712</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>kaposi sarcoma</t>
+          <t>hodgkin lymphoma</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>kidney</t>
+          <t>hypopharynx</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>303</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>larynx</t>
+          <t>in-situ</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>5</v>
+        <v>6184</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>leukemia</t>
+          <t>kaposi sarcoma</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>314</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>lip</t>
+          <t>kidney</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>124</v>
+        <v>303</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>liver</t>
+          <t>larynx</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>85</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>lung</t>
+          <t>leukemia</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>661</v>
+        <v>314</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>melanoma of skin</t>
+          <t>lip, oral cavity</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1611</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>mesothelioma</t>
+          <t>liver</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>31</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>multiple myeloma</t>
+          <t>lung</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>213</v>
+        <v>661</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>nasopharynx</t>
+          <t>melanoma of skin</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>5</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>non-Hodgkin lymphoma</t>
+          <t>mesothelioma</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>583</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>oesophagus</t>
+          <t>multiple myeloma</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>129</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>oropharynx</t>
+          <t>nasopharynx</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>38</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>ovary</t>
+          <t>non-Hodgkin lymphoma</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>801</v>
+        <v>583</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>pancreas</t>
+          <t>oesophagus</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>274</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>salivary glands</t>
+          <t>oropharynx</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>stomach</t>
+          <t>ovary</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>104</v>
+        <v>801</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>thyroid</t>
+          <t>pancreas</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>317</v>
+        <v>274</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>unknown/uncertain</t>
+          <t>salivary glands</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>604</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>vagina</t>
+          <t>stomach</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>18</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>thyroid</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>unknown/uncertain</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>vagina</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
           <t>vulva</t>
         </is>
       </c>
-      <c r="B34" t="n">
+      <c r="B37" t="n">
         <v>64</v>
       </c>
     </row>
@@ -2592,7 +2670,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>27239</v>
+        <v>27332</v>
       </c>
     </row>
     <row r="3">
@@ -2602,7 +2680,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4">
@@ -2612,7 +2690,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2235</v>
+        <v>2547</v>
       </c>
     </row>
     <row r="5">
@@ -2622,7 +2700,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>163</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6">
@@ -2652,7 +2730,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3571</v>
+        <v>3700</v>
       </c>
     </row>
     <row r="9">
@@ -2702,7 +2780,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14">
@@ -2833,7 +2911,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4">
@@ -2883,7 +2961,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1346</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="9">
@@ -2913,7 +2991,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="12">
@@ -3034,19 +3112,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>83.23999999999999</v>
+        <v>83.31999999999999</v>
       </c>
       <c r="C2" t="n">
-        <v>81.79000000000001</v>
+        <v>81.90000000000001</v>
       </c>
       <c r="D2" t="n">
-        <v>85.45</v>
+        <v>85.54000000000001</v>
       </c>
       <c r="E2" t="n">
-        <v>87.5</v>
+        <v>87.44</v>
       </c>
       <c r="F2" t="n">
-        <v>63.2</v>
+        <v>63.23</v>
       </c>
     </row>
     <row r="3">
@@ -3056,19 +3134,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.02</v>
+        <v>0.96</v>
       </c>
       <c r="C3" t="n">
-        <v>0.67</v>
+        <v>0.52</v>
       </c>
       <c r="D3" t="n">
-        <v>0.84</v>
+        <v>0.73</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.66</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="4">
@@ -3090,7 +3168,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>17.29</v>
+        <v>17.3</v>
       </c>
     </row>
     <row r="5">
@@ -3144,13 +3222,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.32</v>
+        <v>1.33</v>
       </c>
       <c r="C7" t="n">
         <v>1.25</v>
       </c>
       <c r="D7" t="n">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -3166,19 +3244,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>9.92</v>
+        <v>9.890000000000001</v>
       </c>
       <c r="C8" t="n">
-        <v>9.529999999999999</v>
+        <v>9.539999999999999</v>
       </c>
       <c r="D8" t="n">
-        <v>7.1</v>
+        <v>7.11</v>
       </c>
       <c r="E8" t="n">
-        <v>7.43</v>
+        <v>7.42</v>
       </c>
       <c r="F8" t="n">
-        <v>12.53</v>
+        <v>12.54</v>
       </c>
     </row>
     <row r="9">
@@ -3232,16 +3310,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2.61</v>
+        <v>2.62</v>
       </c>
       <c r="C11" t="n">
-        <v>4.88</v>
+        <v>4.89</v>
       </c>
       <c r="D11" t="n">
         <v>4.63</v>
       </c>
       <c r="E11" t="n">
-        <v>5.08</v>
+        <v>5.14</v>
       </c>
       <c r="F11" t="n">
         <v>0.05</v>
@@ -3301,7 +3379,7 @@
         <v>0.05</v>
       </c>
       <c r="C14" t="n">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
       <c r="D14" t="n">
         <v>0.26</v>

</xml_diff>